<commit_message>
added destribution by photo,video
</commit_message>
<xml_diff>
--- a/test_subs.xlsx
+++ b/test_subs.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Почта</t>
+    <t xml:space="preserve">ФИО</t>
   </si>
   <si>
     <t xml:space="preserve">Название подписки</t>
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Срок</t>
   </si>
   <si>
-    <t xml:space="preserve">yghjhfcg@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Тест</t>
+    <t xml:space="preserve">Ruslan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub1</t>
   </si>
 </sst>
 </file>
@@ -47,7 +47,7 @@
   <fonts count="5">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -56,24 +56,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -153,60 +150,231 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1f497d"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="eeece1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4f81bd"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="c0504d"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9bbb59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064a2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4bacc6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="f79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ff"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>1</v>
+      <c r="F2" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="yghjhfcg@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>